<commit_message>
Reorganized, upgraded sound effects
</commit_message>
<xml_diff>
--- a/Project2/map/map_stage2.xlsx
+++ b/Project2/map/map_stage2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JumpKing\Project2\map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D4721E-670A-4664-A2BC-BFBF5BF71914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D2AED8-B47B-4E30-8D5A-A430BEC472A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{48E8A6F0-D45C-499F-B0E9-10C3D3B96F46}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{48E8A6F0-D45C-499F-B0E9-10C3D3B96F46}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -531,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7174F57D-9AE7-43AF-99BF-E0807E6314AC}">
   <dimension ref="A1:AN300"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="48" workbookViewId="0">
       <selection activeCell="AN300" sqref="A1:AN300"/>
     </sheetView>
   </sheetViews>
@@ -21321,7 +21321,7 @@
         <v>0</v>
       </c>
       <c r="O171" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P171" s="1">
         <v>2</v>

</xml_diff>